<commit_message>
big impact TN4 Model update
</commit_message>
<xml_diff>
--- a/challenge/TitanicCompetitionV2/Exps.xlsx
+++ b/challenge/TitanicCompetitionV2/Exps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3rd\ML\SGU25-Basic-ML\TitanicCompetitionV2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3rd\ML\sgu2025-2026_ML_basic_nhom3changlinhngulam\challenge\TitanicCompetitionV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A2CCF6-DF93-49E8-B2A6-4C1CB7E2D7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C54B6-6D15-439A-B287-646D75815121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD94E43-75D6-48D1-B4BD-E57EC3AA804D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -108,13 +108,43 @@
   </si>
   <si>
     <t>tn2_GB.csv</t>
+  </si>
+  <si>
+    <t>Name data file</t>
+  </si>
+  <si>
+    <t>train_Labels.xlsx, test_Labels.xlsx</t>
+  </si>
+  <si>
+    <t>combined_Onehot.csv</t>
+  </si>
+  <si>
+    <t>combined_OnehotV2.csv</t>
+  </si>
+  <si>
+    <t>24/10/2025</t>
+  </si>
+  <si>
+    <t>24/10/2026</t>
+  </si>
+  <si>
+    <t>tn3_OHtunning.ipynb</t>
+  </si>
+  <si>
+    <t>Out of turn</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +199,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -238,13 +280,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -256,33 +329,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -290,18 +336,51 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -638,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5144BD18-B6E8-4F53-8753-F1152E2A01F4}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,11 +731,12 @@
     <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="27.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="47" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -678,13 +758,16 @@
       <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="H1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -699,13 +782,16 @@
       <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="11"/>
+      <c r="H2" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -718,11 +804,12 @@
       <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
@@ -735,11 +822,12 @@
       <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
@@ -752,19 +840,20 @@
       <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="8">
         <v>0.75836999999999999</v>
       </c>
       <c r="E6" s="4">
@@ -773,17 +862,20 @@
       <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="16" t="s">
+      <c r="H6" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="8">
         <v>0.78468000000000004</v>
       </c>
       <c r="E7" s="4">
@@ -792,15 +884,16 @@
       <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="16" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="8">
         <v>0.77032999999999996</v>
       </c>
       <c r="E8" s="4">
@@ -809,15 +902,16 @@
       <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="18" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="8">
         <v>0.76793999999999996</v>
       </c>
       <c r="E9" s="4">
@@ -826,28 +920,159 @@
       <c r="F9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.78229000000000004</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.78229000000000004</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.82040000000000002</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="4">
+        <v>0.81930000000000003</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.75358000000000003</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="A10:A13"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="G2:G5"/>
@@ -855,6 +1080,7 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="G6:G9"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{DA80437C-3527-4D0F-8C08-64F21AEE74A7}"/>
     <hyperlink ref="D3" r:id="rId2" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{DFD1ADC3-E68B-4A7C-93C8-D5F11F022379}"/>
@@ -863,8 +1089,11 @@
     <hyperlink ref="D7" r:id="rId5" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{D8B27F99-2A80-4C63-A822-4E680F67E119}"/>
     <hyperlink ref="D8" r:id="rId6" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{F8DAD611-8E82-449E-BD63-43F2C93C2A63}"/>
     <hyperlink ref="D9" r:id="rId7" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{0BCF4FCD-F25A-42F3-88AE-8B7C4E147D57}"/>
+    <hyperlink ref="D13" r:id="rId8" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{C62B51E0-7C7A-4C5F-B71F-E6A91D0AF10B}"/>
+    <hyperlink ref="D10" r:id="rId9" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{56B323A2-942A-4A12-A3F5-BFC3765E2BB0}"/>
+    <hyperlink ref="D11" r:id="rId10" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{4BCA9ACC-4BD7-4541-81DE-E0902FF54F34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   challenge/TitanicCompetitionV2/Exps.xlsx 	new file:   challenge/TitanicCompetitionV2/proves/tn4/567601584_1540538620291665_2102899905599654477_n.png
</commit_message>
<xml_diff>
--- a/challenge/TitanicCompetitionV2/Exps.xlsx
+++ b/challenge/TitanicCompetitionV2/Exps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3rd\ML\sgu2025-2026_ML_basic_nhom3changlinhngulam\challenge\TitanicCompetitionV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C54B6-6D15-439A-B287-646D75815121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73657005-1010-41D9-A8D6-C47D97B4AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CDD94E43-75D6-48D1-B4BD-E57EC3AA804D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -125,26 +125,29 @@
     <t>24/10/2025</t>
   </si>
   <si>
-    <t>24/10/2026</t>
-  </si>
-  <si>
-    <t>tn3_OHtunning.ipynb</t>
-  </si>
-  <si>
-    <t>Out of turn</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>null</t>
+    <t>29/10/2025</t>
+  </si>
+  <si>
+    <t>tn4_final.ipynb</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>SVM.csv</t>
+  </si>
+  <si>
+    <t>Tunned SVM, StandalizeScaler,OneHot Encoder</t>
+  </si>
+  <si>
+    <t>train_final.csv, test_final.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,16 +203,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,69 +328,71 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -398,6 +411,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>30234</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Hình ảnh 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F40868FE-A8AB-7E27-CD1F-38F07110749D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2811072"/>
+          <a:ext cx="6450084" cy="532339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -720,7 +782,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,337 +799,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="16">
         <v>0.78708</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="17">
         <v>0.79900000000000004</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="16">
         <v>0.78708</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="17">
         <v>0.79100000000000004</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="16">
         <v>0.73923000000000005</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="17">
         <v>0.81579999999999997</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="16">
         <v>0.76554999999999995</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="17">
         <v>0.82369999999999999</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="24">
         <v>0.75836999999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="17">
         <v>0.81479999999999997</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="7" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="24">
         <v>0.78468000000000004</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="17">
         <v>0.81259999999999999</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="24">
         <v>0.77032999999999996</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="17">
         <v>0.81030000000000002</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="24">
         <v>0.76793999999999996</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="17">
         <v>0.82709999999999995</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="24">
         <v>0.78229000000000004</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="17">
         <v>0.81820000000000004</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="23" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="7" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="24">
         <v>0.78229000000000004</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="25">
         <v>0.82040000000000002</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="23"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4">
+      <c r="D12" s="26">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="E12" s="17">
         <v>0.81930000000000003</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="23"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="9" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="24">
         <v>0.75358000000000003</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="17">
         <v>0.83840000000000003</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="23"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="23" t="s">
-        <v>27</v>
+      <c r="C14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="28">
+        <v>0.79186000000000001</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="23"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="23"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="23"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="H14:H17"/>
+  <mergeCells count="11">
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
@@ -1080,7 +1125,7 @@
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="G6:G9"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{DA80437C-3527-4D0F-8C08-64F21AEE74A7}"/>
     <hyperlink ref="D3" r:id="rId2" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{DFD1ADC3-E68B-4A7C-93C8-D5F11F022379}"/>
@@ -1092,8 +1137,11 @@
     <hyperlink ref="D13" r:id="rId8" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{C62B51E0-7C7A-4C5F-B71F-E6A91D0AF10B}"/>
     <hyperlink ref="D10" r:id="rId9" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{56B323A2-942A-4A12-A3F5-BFC3765E2BB0}"/>
     <hyperlink ref="D11" r:id="rId10" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{4BCA9ACC-4BD7-4541-81DE-E0902FF54F34}"/>
+    <hyperlink ref="D14" r:id="rId11" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{68C1677E-193E-4979-AA77-25CC43B5EDA6}"/>
+    <hyperlink ref="D12" r:id="rId12" display="https://www.kaggle.com/competitions/titanic/submissions" xr:uid="{560A083C-6DC7-4B55-A2EB-3594CD1C31CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>